<commit_message>
Comparaison faite pour le Libelle, le state, et la gravite sortie sur la console
</commit_message>
<xml_diff>
--- a/QueryResult.xlsx
+++ b/QueryResult.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2215" uniqueCount="1398">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2222" uniqueCount="1400">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -11638,6 +11638,12 @@
 46003	02/03/1917	31/01/2019	46002	46004	
 </t>
   </si>
+  <si>
+    <t xml:space="preserve">CNAM_00327721</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[MODE LOT 3 - IT 1.3] -TEST</t>
+  </si>
 </sst>
 </file>
 
@@ -11651,6 +11657,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -11676,12 +11683,19 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
   </borders>
@@ -11710,13 +11724,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -11736,13 +11754,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H277"/>
+  <dimension ref="A1:H278"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A263" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E288" activeCellId="0" sqref="E288"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -18942,6 +18963,29 @@
       </c>
       <c r="H277" s="1" t="s">
         <v>1397</v>
+      </c>
+    </row>
+    <row r="278" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A278" s="2" t="s">
+        <v>1398</v>
+      </c>
+      <c r="B278" s="2" t="s">
+        <v>1399</v>
+      </c>
+      <c r="C278" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="D278" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E278" s="2" t="s">
+        <v>1395</v>
+      </c>
+      <c r="F278" s="2" t="s">
+        <v>1396</v>
+      </c>
+      <c r="G278" s="2" t="s">
+        <v>658</v>
       </c>
     </row>
   </sheetData>

</xml_diff>